<commit_message>
100 smartphone, updated rankings
</commit_message>
<xml_diff>
--- a/_resources/_rankings.xlsx
+++ b/_resources/_rankings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blubu\Documents\Coding\oii2021\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\oii2021\_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7A696B-BAAC-4B3B-98D9-F00EEEE2856B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91967B5A-273B-4A84-8E0A-81C750726F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,10 +167,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$76</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="75"/>
                 <c:pt idx="0">
                   <c:v>44306</c:v>
                 </c:pt>
@@ -245,16 +245,166 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>44330</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44331</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44332</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>44333</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>44334</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44335</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44336</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44337</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>44338</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>44339</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>44340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44341</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44342</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44343</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>44344</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44345</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44346</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>44347</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44349</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44350</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44351</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44352</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44353</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>44354</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>44355</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>44356</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>44357</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44358</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44359</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>44360</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>44361</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>44362</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>44363</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>44364</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>44365</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>44366</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>44367</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>44368</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>44369</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>44370</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>44371</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>44372</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>44373</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>44374</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>44375</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>44376</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>44377</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44379</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>44380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:f>Sheet1!$B$2:$B$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="75"/>
                 <c:pt idx="0">
                   <c:v>53</c:v>
                 </c:pt>
@@ -329,6 +479,120 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,19 +1627,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44306</v>
       </c>
@@ -1397,7 +1661,7 @@
         <v>-2317</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44307</v>
       </c>
@@ -1408,7 +1672,7 @@
         <v>-1873</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44308</v>
       </c>
@@ -1419,7 +1683,7 @@
         <v>-1873</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44309</v>
       </c>
@@ -1430,7 +1694,7 @@
         <v>-1873</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44310</v>
       </c>
@@ -1441,7 +1705,7 @@
         <v>-1873</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44311</v>
       </c>
@@ -1452,7 +1716,7 @@
         <v>-1723</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44312</v>
       </c>
@@ -1463,7 +1727,7 @@
         <v>-1723</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44313</v>
       </c>
@@ -1474,7 +1738,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44314</v>
       </c>
@@ -1485,7 +1749,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44315</v>
       </c>
@@ -1496,7 +1760,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44316</v>
       </c>
@@ -1507,7 +1771,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44317</v>
       </c>
@@ -1518,7 +1782,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44318</v>
       </c>
@@ -1529,7 +1793,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44319</v>
       </c>
@@ -1540,7 +1804,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44320</v>
       </c>
@@ -1551,7 +1815,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44321</v>
       </c>
@@ -1562,7 +1826,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44322</v>
       </c>
@@ -1573,7 +1837,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44323</v>
       </c>
@@ -1584,7 +1848,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44324</v>
       </c>
@@ -1595,7 +1859,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44325</v>
       </c>
@@ -1606,7 +1870,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44326</v>
       </c>
@@ -1617,7 +1881,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44327</v>
       </c>
@@ -1628,7 +1892,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44328</v>
       </c>
@@ -1639,7 +1903,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44329</v>
       </c>
@@ -1650,7 +1914,7 @@
         <v>-1553</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44330</v>
       </c>
@@ -1659,6 +1923,609 @@
       </c>
       <c r="C26">
         <v>-1482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44331</v>
+      </c>
+      <c r="B27">
+        <v>106</v>
+      </c>
+      <c r="C27">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44332</v>
+      </c>
+      <c r="B28">
+        <v>106</v>
+      </c>
+      <c r="C28">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>44333</v>
+      </c>
+      <c r="B29">
+        <v>106</v>
+      </c>
+      <c r="C29">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44334</v>
+      </c>
+      <c r="B30">
+        <v>106</v>
+      </c>
+      <c r="C30">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44335</v>
+      </c>
+      <c r="B31">
+        <v>106</v>
+      </c>
+      <c r="C31">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44336</v>
+      </c>
+      <c r="B32">
+        <v>106</v>
+      </c>
+      <c r="C32">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>44337</v>
+      </c>
+      <c r="B33">
+        <v>106</v>
+      </c>
+      <c r="C33">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>44338</v>
+      </c>
+      <c r="B34">
+        <v>106</v>
+      </c>
+      <c r="C34">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B35">
+        <v>106</v>
+      </c>
+      <c r="C35">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B36">
+        <v>106</v>
+      </c>
+      <c r="C36">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B37">
+        <v>106</v>
+      </c>
+      <c r="C37">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>44342</v>
+      </c>
+      <c r="B38">
+        <v>106</v>
+      </c>
+      <c r="C38">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B39">
+        <v>106</v>
+      </c>
+      <c r="C39">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B40">
+        <v>106</v>
+      </c>
+      <c r="C40">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>44345</v>
+      </c>
+      <c r="B41">
+        <v>106</v>
+      </c>
+      <c r="C41">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B42">
+        <v>106</v>
+      </c>
+      <c r="C42">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>44347</v>
+      </c>
+      <c r="B43">
+        <v>106</v>
+      </c>
+      <c r="C43">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B44">
+        <v>106</v>
+      </c>
+      <c r="C44">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B45">
+        <v>106</v>
+      </c>
+      <c r="C45">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B46">
+        <v>106</v>
+      </c>
+      <c r="C46">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B47">
+        <v>106</v>
+      </c>
+      <c r="C47">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B48">
+        <v>106</v>
+      </c>
+      <c r="C48">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>44353</v>
+      </c>
+      <c r="B49">
+        <v>106</v>
+      </c>
+      <c r="C49">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B50">
+        <v>106</v>
+      </c>
+      <c r="C50">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B51">
+        <v>106</v>
+      </c>
+      <c r="C51">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B52">
+        <v>106</v>
+      </c>
+      <c r="C52">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B53">
+        <v>106</v>
+      </c>
+      <c r="C53">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B54">
+        <v>106</v>
+      </c>
+      <c r="C54">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>44359</v>
+      </c>
+      <c r="B55">
+        <v>106</v>
+      </c>
+      <c r="C55">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>44360</v>
+      </c>
+      <c r="B56">
+        <v>106</v>
+      </c>
+      <c r="C56">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B57">
+        <v>106</v>
+      </c>
+      <c r="C57">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B58">
+        <v>106</v>
+      </c>
+      <c r="C58">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B59">
+        <v>106</v>
+      </c>
+      <c r="C59">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B60">
+        <v>106</v>
+      </c>
+      <c r="C60">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B61">
+        <v>106</v>
+      </c>
+      <c r="C61">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>44366</v>
+      </c>
+      <c r="B62">
+        <v>106</v>
+      </c>
+      <c r="C62">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>44367</v>
+      </c>
+      <c r="B63">
+        <v>106</v>
+      </c>
+      <c r="C63">
+        <v>-1482</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B64">
+        <v>129</v>
+      </c>
+      <c r="C64">
+        <v>-1326</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>44369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>44370</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>44371</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>44372</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>44373</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>44374</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>44375</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>44376</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>44379</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>44380</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>44381</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>44382</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>44383</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>44384</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>44385</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>44386</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>44387</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>44388</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>44389</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>44390</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>44391</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>44392</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>44393</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>44394</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>44395</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>44396</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>44397</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>44398</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>44399</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>44401</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>44402</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>44403</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>44404</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>44405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>